<commit_message>
Creates visualisation for clefts
</commit_message>
<xml_diff>
--- a/data/ESLO/où_questions.xlsx
+++ b/data/ESLO/où_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinabonan/Desktop/GitHubRepos/parameters-corpus-work/data/ESLO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E617856-94D1-5846-B7E8-B48AA8CCD1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCC3CB-03BC-9647-A213-41FA43FFD672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-68800" yWindow="-10300" windowWidth="29240" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6683" uniqueCount="1578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6691" uniqueCount="1578">
   <si>
     <t>recherche</t>
   </si>
@@ -17083,10 +17083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF739"/>
+  <dimension ref="A1:BH739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA4" zoomScale="114" workbookViewId="0">
-      <selection activeCell="AD67" sqref="AD67:AF69"/>
+    <sheetView tabSelected="1" topLeftCell="AP27" zoomScale="114" workbookViewId="0">
+      <selection activeCell="BH65" sqref="BH65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17095,7 +17095,7 @@
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -17127,7 +17127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -17159,7 +17159,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -17191,7 +17191,7 @@
         <v>1430386</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -17223,7 +17223,7 @@
         <v>2424703</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -17255,7 +17255,7 @@
         <v>66273</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -17287,7 +17287,7 @@
         <v>1015263</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -17319,7 +17319,7 @@
         <v>2290143</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -17351,7 +17351,7 @@
         <v>1881173</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -17383,7 +17383,7 @@
         <v>2002487</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -17415,7 +17415,7 @@
         <v>2838929</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -17450,7 +17450,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -17482,7 +17482,7 @@
         <v>4129669</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -17520,7 +17520,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -17566,8 +17566,17 @@
       <c r="AF14">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="BF14" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -17613,8 +17622,17 @@
       <c r="AF15">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="BF15" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -18742,7 +18760,7 @@
         <v>5455792</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -18774,7 +18792,7 @@
         <v>5724292</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -18806,7 +18824,7 @@
         <v>1531163</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -18838,7 +18856,7 @@
         <v>2366551</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -18870,7 +18888,7 @@
         <v>3498276</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -18902,7 +18920,7 @@
         <v>1328672</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -18934,7 +18952,7 @@
         <v>2814167</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -18966,7 +18984,7 @@
         <v>91686</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -18998,7 +19016,7 @@
         <v>2958200</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -19030,7 +19048,7 @@
         <v>2960164</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -19062,7 +19080,7 @@
         <v>2961272</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -19094,7 +19112,7 @@
         <v>5305103</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -19126,7 +19144,7 @@
         <v>5371402</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -19158,7 +19176,7 @@
         <v>223029</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -19190,7 +19208,7 @@
         <v>995955</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -19225,7 +19243,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -19256,8 +19274,17 @@
       <c r="J64">
         <v>1876757</v>
       </c>
-    </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="BF64" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG64" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -19294,8 +19321,17 @@
       <c r="P65" t="s">
         <v>1576</v>
       </c>
-    </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="BF65" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG65" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH65">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -19342,7 +19378,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -19389,7 +19425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -19436,7 +19472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -19483,7 +19519,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -19521,7 +19557,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -19559,7 +19595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -19597,7 +19633,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -19635,7 +19671,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -19673,7 +19709,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -19711,7 +19747,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -19743,7 +19779,7 @@
         <v>4082348</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -19775,7 +19811,7 @@
         <v>20777</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -19807,7 +19843,7 @@
         <v>3859315</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -19839,7 +19875,7 @@
         <v>69853</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1</v>
       </c>

</xml_diff>